<commit_message>
Erweiterung Arbeitspaket-Liste und erste Schritte in MS Project
</commit_message>
<xml_diff>
--- a/Arbeitspakete_Liste_NEU.xlsx
+++ b/Arbeitspakete_Liste_NEU.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98CF45BB-C612-4A86-AE63-B0C9A000EABF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{288DA868-7132-446D-97D2-84C911889F17}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4005" yWindow="3615" windowWidth="18900" windowHeight="11055" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
   <si>
     <t>Nr.</t>
   </si>
@@ -141,6 +141,9 @@
   </si>
   <si>
     <t>Fehlerbhebung bei/nach Rollout</t>
+  </si>
+  <si>
+    <t>Berechtigungskonzept erstellen</t>
   </si>
 </sst>
 </file>
@@ -516,10 +519,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+      <selection activeCell="A2" sqref="A2:A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -599,26 +602,27 @@
       <c r="E5" s="3"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>26</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="C6" s="8"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
+      <c r="I6" s="1"/>
     </row>
     <row r="7" spans="1:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
+      <c r="A7" s="4">
+        <v>6</v>
+      </c>
       <c r="B7" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>28</v>
+        <v>9</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>26</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
@@ -628,36 +632,36 @@
         <v>7</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>8</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>9</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
@@ -667,10 +671,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>30</v>
+        <v>2</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>29</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -680,7 +684,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>30</v>
@@ -693,9 +697,11 @@
         <v>12</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="6"/>
+        <v>13</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>30</v>
+      </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
     </row>
@@ -704,11 +710,9 @@
         <v>13</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>33</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="C14" s="6"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
     </row>
@@ -717,10 +721,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -730,9 +734,11 @@
         <v>15</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" s="6"/>
+        <v>16</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>25</v>
+      </c>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
     </row>
@@ -741,7 +747,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C17" s="6"/>
       <c r="D17" s="3"/>
@@ -752,7 +758,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C18" s="6"/>
       <c r="D18" s="3"/>
@@ -763,11 +769,22 @@
         <v>18</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C19" s="6"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="4">
+        <v>19</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="6"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Arbeitpakete gereviewed, Listen aktualisiert
</commit_message>
<xml_diff>
--- a/Arbeitspakete_Liste_NEU.xlsx
+++ b/Arbeitspakete_Liste_NEU.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F016591-A66D-4BDD-95A7-B197DEFCBB49}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0EE3FCD-A47C-47D5-8982-BFCD669A5B5D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24840" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="63">
   <si>
     <t>Nr.</t>
   </si>
@@ -242,6 +242,9 @@
   </si>
   <si>
     <t>besprochen</t>
+  </si>
+  <si>
+    <t>Projektmanagement durchführen</t>
   </si>
 </sst>
 </file>
@@ -271,7 +274,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -342,11 +345,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -386,6 +400,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -712,25 +729,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="59.5546875" customWidth="1"/>
-    <col min="4" max="4" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="30.33203125" customWidth="1"/>
+    <col min="1" max="1" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="59.5703125" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30.28515625" customWidth="1"/>
     <col min="8" max="8" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -751,7 +768,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -771,7 +788,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -789,7 +806,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -801,13 +818,13 @@
         <v>34</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G4" s="10">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -820,13 +837,15 @@
       <c r="D5" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E5" s="3"/>
+      <c r="E5" s="3" t="s">
+        <v>61</v>
+      </c>
       <c r="G5" s="10">
         <v>10</v>
       </c>
       <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -837,13 +856,15 @@
       <c r="D6" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E6" s="3"/>
+      <c r="E6" s="3" t="s">
+        <v>61</v>
+      </c>
       <c r="G6" s="10">
         <v>3</v>
       </c>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -864,7 +885,7 @@
       </c>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -875,13 +896,15 @@
       <c r="D8" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E8" s="3"/>
+      <c r="E8" s="3" t="s">
+        <v>61</v>
+      </c>
       <c r="G8" s="10" t="s">
         <v>58</v>
       </c>
       <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -892,13 +915,15 @@
       <c r="D9" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E9" s="3"/>
+      <c r="E9" s="3" t="s">
+        <v>61</v>
+      </c>
       <c r="G9" s="10" t="s">
         <v>58</v>
       </c>
       <c r="H9" s="1"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -909,13 +934,15 @@
       <c r="D10" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E10" s="3"/>
+      <c r="E10" s="3" t="s">
+        <v>61</v>
+      </c>
       <c r="G10" s="10" t="s">
         <v>58</v>
       </c>
       <c r="H10" s="1"/>
     </row>
-    <row r="11" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -935,7 +962,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -955,7 +982,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -968,12 +995,14 @@
       <c r="D13" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E13" s="3"/>
+      <c r="E13" s="3" t="s">
+        <v>61</v>
+      </c>
       <c r="G13" s="11" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -987,13 +1016,13 @@
         <v>34</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G14" s="11" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -1006,12 +1035,14 @@
       <c r="D15" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E15" s="3"/>
+      <c r="E15" s="3" t="s">
+        <v>61</v>
+      </c>
       <c r="G15" s="11" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -1031,7 +1062,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -1044,12 +1075,14 @@
       <c r="D17" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="E17" s="3"/>
+      <c r="E17" s="3" t="s">
+        <v>61</v>
+      </c>
       <c r="G17" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -1061,13 +1094,13 @@
         <v>34</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G18" s="10" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -1081,13 +1114,13 @@
         <v>34</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G19" s="10" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -1101,13 +1134,13 @@
         <v>35</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G20" s="10" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -1125,7 +1158,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -1137,13 +1170,13 @@
         <v>34</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G22" s="10" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -1155,13 +1188,13 @@
         <v>34</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G23" s="10" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -1173,10 +1206,15 @@
         <v>35</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G24" s="10" t="s">
         <v>57</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B25" s="14" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1220,17 +1258,17 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -1238,7 +1276,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>37</v>
       </c>
@@ -1246,7 +1284,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>36</v>
       </c>

</xml_diff>